<commit_message>
fixed some issues of import (dead_injured, house_damage)
</commit_message>
<xml_diff>
--- a/templates/deadinjured.xlsx
+++ b/templates/deadinjured.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">Date Of Report  </t>
   </si>
   <si>
-    <t>Halqa Patwari</t>
-  </si>
-  <si>
     <t>Medical Officer</t>
   </si>
   <si>
@@ -69,6 +66,42 @@
   </si>
   <si>
     <t>Counter signed by DC</t>
+  </si>
+  <si>
+    <t>Patwari</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Father Name 1</t>
+  </si>
+  <si>
+    <t>Address of affectee</t>
+  </si>
+  <si>
+    <t>Peshawar</t>
+  </si>
+  <si>
+    <t>Some Reason</t>
+  </si>
+  <si>
+    <t>2012-03-02</t>
+  </si>
+  <si>
+    <t>2015-31-04</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Father Name 2</t>
+  </si>
+  <si>
+    <t>injured</t>
   </si>
 </sst>
 </file>
@@ -104,9 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,10 +432,11 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
     <col min="14" max="14" width="24.7109375" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" customWidth="1"/>
   </cols>
@@ -431,26 +466,120 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>12234123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>12234123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing Process - 1a
</commit_message>
<xml_diff>
--- a/templates/deadinjured.xlsx
+++ b/templates/deadinjured.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>injured</t>
+  </si>
+  <si>
+    <t>Relief Amount</t>
   </si>
 </sst>
 </file>
@@ -421,27 +424,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,34 +466,37 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -510,18 +518,18 @@
       <c r="G2">
         <v>1000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
@@ -534,8 +542,11 @@
       <c r="O2" t="s">
         <v>22</v>
       </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -555,20 +566,20 @@
         <v>19</v>
       </c>
       <c r="G3">
+        <v>2000</v>
+      </c>
+      <c r="H3">
         <v>1000</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
       <c r="L3" t="s">
         <v>22</v>
       </c>
@@ -579,6 +590,9 @@
         <v>22</v>
       </c>
       <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>